<commit_message>
Actualizacion para uso de Openai y Groq
Ahora existe la posibilidad de utilizar gpt-4o-mini y openai de embeddings, por parte de groq no existe modelo para embeddings por lo que si se usa ese modelo se hará el embedding de mistral, pero la parte de groq hace falta hacerle ajustes ya que no se parece la manera de llamar al modelo respecto a mistral u openai
</commit_message>
<xml_diff>
--- a/resultados.xlsx
+++ b/resultados.xlsx
@@ -2,15 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Resultados" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -50,7 +49,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -413,13 +412,17 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG4"/>
+  <dimension ref="A1:AG16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25"/>
+  <cols>
+    <col width="31.53125" customWidth="1" min="2" max="2"/>
+    <col width="30.86328125" customWidth="1" min="3" max="3"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -1078,6 +1081,1986 @@
         </is>
       </c>
       <c r="AG4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2022-2-DiamondD-Report.pdf</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>mistral-large-latest</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>1973</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>Trabajaban en cubierta tratando de desencruzar los cables de remolque.</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>Un bote salvavidas de la RNLI.</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>El propietario recogió varios chalecos salvavidas, una caja de bengalas y una pequeña bolsa personal que contenía medicamentos y ropa seca.</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X5" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="Y5" t="inlineStr">
+        <is>
+          <t>2 personas; el patrón y el dueño.</t>
+        </is>
+      </c>
+      <c r="Z5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AA5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AB5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AC5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AD5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AE5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AF5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AG5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2022-2-DiamondD-Report.pdf</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>gpt-4o-mini</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>1500</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>A 38-year-old UK national</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>North Shields, England</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>1973</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>Fine and dry with light airs</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>The crew was attempting to uncross the towing wires while hauling in the trawl gear.</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>RNLI (Royal National Lifeboat Institution) lifeboat</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>From the liferaft and the main deck.</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>Yes, the crew contacted Humber coastguard to request assistance.</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>Yes, the vessel had previously run aground and suffered damage to its bow in 2014.</t>
+        </is>
+      </c>
+      <c r="V6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X6" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="Y6" t="inlineStr">
+        <is>
+          <t>2 (the skipper and the owner)</t>
+        </is>
+      </c>
+      <c r="Z6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AA6" t="inlineStr">
+        <is>
+          <t>0 hours 8 minutes</t>
+        </is>
+      </c>
+      <c r="AB6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AC6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AD6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AE6" t="inlineStr">
+        <is>
+          <t>1.5</t>
+        </is>
+      </c>
+      <c r="AF6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AG6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2022-2-DiamondD-Report.pdf</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>gpt-4o-mini</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>1500</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>The owner is a 38-year-old UK national.</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>The vessel was heading to North Shields, England.</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>1973</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>Fine and dry with light airs</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>Attempting to uncross towing wires and haul in the trawl net</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>RNLI lifeboat</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>The crew member retrieved safety equipment from the liferaft, which included lifejackets, a box of flares, and personal items.</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>Yes, the skipper made a VHF radio call to Humber coastguard at 1453 to request assistance.</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>Yes, on 24 May 2014, Diamond D suffered damage to its bow when it ran aground.</t>
+        </is>
+      </c>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X7" t="inlineStr">
+        <is>
+          <t>1500 GMT</t>
+        </is>
+      </c>
+      <c r="Y7" t="inlineStr">
+        <is>
+          <t>2; the skipper and the owner</t>
+        </is>
+      </c>
+      <c r="Z7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AA7" t="inlineStr">
+        <is>
+          <t>0 hours and 8 minutes</t>
+        </is>
+      </c>
+      <c r="AB7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AC7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AD7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AE7" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="AF7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AG7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2022-2-DiamondD-Report.pdf</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>gpt-4o-mini</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>16 August 2020 at about 1500</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>The owner was a 38-year-old UK national.</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>North Shields, England (intended)</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>1973</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>Yes, a VHF call to alert the coastguard was made.</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>Fine and dry with light airs</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>The owner was operating the main trawl winch and the skipper was monitoring the trawl gear as it was being hauled.</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>RNLI lifeboat</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>The owner grabbed several lifejackets, a box of flares and a small personal bag containing medication and dry clothes and, having tossed them into the liferaft, jumped into it from the main deck.</t>
+        </is>
+      </c>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>At 1359, one of the owner’s relatives contacted the coastguard and advised them that Diamond D was overdue. The skipper reached through an open wheelhouse window and, at 1453, used Diamond D’s main VHF radio to call Humber coastguard on channel 16 and request assistance.</t>
+        </is>
+      </c>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>On 24 May 2014, Diamond D suffered damage to its bow when it ran aground. On 11 August 2014, following extensive repairs, a condition survey was undertaken by an independent surveyor. On 19 September 2019, an insurance valuation survey was carried out.</t>
+        </is>
+      </c>
+      <c r="V8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="W8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X8" t="inlineStr">
+        <is>
+          <t>1500 GMT+1</t>
+        </is>
+      </c>
+      <c r="Y8" t="inlineStr">
+        <is>
+          <t>2 people onboard: the skipper and the owner</t>
+        </is>
+      </c>
+      <c r="Z8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AA8" t="inlineStr">
+        <is>
+          <t>0 hours and 8 minutes</t>
+        </is>
+      </c>
+      <c r="AB8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AC8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AD8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AE8" t="inlineStr">
+        <is>
+          <t>1.5</t>
+        </is>
+      </c>
+      <c r="AF8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AG8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2022-2-DiamondD-Report.pdf</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>gpt-4o-mini</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>16 August 2020 at about 1500</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>The owner was a 38-year-old UK national.</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>The vessel was heading for North Shields, England, for annual maintenance and an out of water survey.</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>The vessel began to slow down and then stopped.</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>1973</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>Fine and dry with light airs</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>The owner was operating the main trawl winch while the skipper went to the transom to monitor the trawl gear as it was being hauled.</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>RNLI lifeboat</t>
+        </is>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>The owner grabbed several lifejackets, a box of flares and a small personal bag containing medication and dry clothes.</t>
+        </is>
+      </c>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>At 1453, the skipper used Diamond D’s main VHF radio to call Humber coastguard on channel 16 and request assistance.</t>
+        </is>
+      </c>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>On 24 May 2014, Diamond D suffered damage to its bow when it ran aground.</t>
+        </is>
+      </c>
+      <c r="V9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="W9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X9" t="inlineStr">
+        <is>
+          <t>1500 GMT+1</t>
+        </is>
+      </c>
+      <c r="Y9" t="inlineStr">
+        <is>
+          <t>2 people: the owner and the skipper</t>
+        </is>
+      </c>
+      <c r="Z9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AA9" t="inlineStr">
+        <is>
+          <t>0 hours and 8 minutes</t>
+        </is>
+      </c>
+      <c r="AB9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AC9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AD9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AE9" t="inlineStr">
+        <is>
+          <t>22 hours</t>
+        </is>
+      </c>
+      <c r="AF9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AG9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2022-2-DiamondD-Report.pdf</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>mistral-large-latest</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>1500: 16 August 2020</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>North Shields, England</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>1973</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>At 1453, the skipper used Diamond D’s main VHF radio to call Humber coastguard on channel 16 and request assistance.</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>The winds were light, the seawater temperature was 13°C and there was very little swell.</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>The skipper remained on watch in the wheelhouse and the owner went to the cabin to get some sleep.</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>Tynemouth all-weather lifeboat (ALB)</t>
+        </is>
+      </c>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="T10" t="inlineStr">
+        <is>
+          <t>At 1453, the skipper used Diamond D’s main VHF radio to call Humber coastguard on channel 16 and request assistance.</t>
+        </is>
+      </c>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="V10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="W10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X10" t="inlineStr">
+        <is>
+          <t>1500</t>
+        </is>
+      </c>
+      <c r="Y10" t="inlineStr">
+        <is>
+          <t>2; the skipper and owner</t>
+        </is>
+      </c>
+      <c r="Z10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AA10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AB10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AC10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AD10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AE10" t="inlineStr">
+        <is>
+          <t>16.5</t>
+        </is>
+      </c>
+      <c r="AF10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AG10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>2022-2-DiamondD-Report.pdf</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>mistral-large-latest</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>At about 1500</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>North Shields, England</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>1973</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>The winds were light, the seawater temperature was 13°C and there was very little swell.</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>The skipper remained on watch in the wheelhouse and the owner went to the cabin to get some sleep.</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>Tynemouth all-weather lifeboat (ALB)</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>At 1453, used Diamond D ’s main VHF radio to call Humber coastguard on channel 16 and request assistance.</t>
+        </is>
+      </c>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="V11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="W11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X11" t="inlineStr">
+        <is>
+          <t>1600</t>
+        </is>
+      </c>
+      <c r="Y11" t="inlineStr">
+        <is>
+          <t>2 people were onboard at the time of the accident, and they were the skipper and owner.</t>
+        </is>
+      </c>
+      <c r="Z11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AA11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AB11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AC11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AD11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AE11" t="inlineStr">
+        <is>
+          <t>17.25</t>
+        </is>
+      </c>
+      <c r="AF11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AG11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>2025-3-Waverley-ReportAndAnnexes.pdf</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>mistral-large-latest</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Time:	1646:21</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>The vessel's owner is Waverley Steam Navigation Co. Limited (WSN).</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>The vessel was heading to Brodick pier.</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Speed:	2.8kts</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>1947</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>At the time of the accident there was a gentle westerly wind of 12kts (force 3), occasionally gusting to 21kts (force 5), and an air temperature of 17.7°C. The weather was sunny with little cloud.</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="T12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="U12" t="inlineStr">
+        <is>
+          <t>Yes, there were previous accidents involving the vessel Waverley. In August 2017, Waverley made contact with the pier at Rothesay in the Firth of Clyde. In June 2009, Waverley made heavy contact with Dunoon pier. In July 2006, Waverley grounded briefly on departure from Girvan Harbour, Scotland. In October 2004, the WEL passenger vessel Balmoral grounded on the Dagger Reef, Gower Peninsula, Wales. In June 2004, Waverley grounded on the edge of Boiler Reef, south of Sanda Island, Scotland.</t>
+        </is>
+      </c>
+      <c r="V12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="W12" t="inlineStr">
+        <is>
+          <t>The crew were practised in berthing at Brodick. The manual handling characteristics of Waverley required careful control of speed and engine state during berthing manoeuvres and the on-watch engineer was vital to any change in the provision of propulsion. However, it was noted that the crew might have been better prepared had sufficient warning been given.</t>
+        </is>
+      </c>
+      <c r="X12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Y12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Z12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AA12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AB12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AC12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AD12" t="inlineStr">
+        <is>
+          <t>Yes, the speed reduced from 14.0kts to 2.8kts, a 80% decrease.</t>
+        </is>
+      </c>
+      <c r="AE12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AF12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AG12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>2025-3-Waverley-ReportAndAnnexes.pdf</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>mistral-large-latest</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>1646:21</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Waverley Steam Navigation Co. Limited (WSN)</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Brodick pier, Isle of Arran, Scotland</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>2.8kts</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>1947</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>At the time of the accident there was a gentle westerly wind of 12kts (force 3), occasionally gusting to 21kts (force 5), and an air temperature of 17.7°C. High tide was 2.98m at 1409 and the predicted low tide was 0.63m at 1924. There was a slight southerly tidal stream of about 0.1kts in the bay. The weather was sunny with little cloud.</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>The master in command at the time of the accident had extensive paddle steamer experience and had worked on Waverley for 26 years, including 6 years as the senior master and another 14 years as master or relief master.</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="T13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>Yes, there were several previous accidents involving the vessel Waverley.</t>
+        </is>
+      </c>
+      <c r="V13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="W13" t="inlineStr">
+        <is>
+          <t>The vessel's crew was professional seafarers, but there was limited documented training provided beyond the safety induction and the management of specific hazards such as a fire on board. Training was reliant on the supervision and assurance provided by more experienced people.</t>
+        </is>
+      </c>
+      <c r="X13" t="inlineStr">
+        <is>
+          <t>1646</t>
+        </is>
+      </c>
+      <c r="Y13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Z13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AA13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AB13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AC13" t="inlineStr">
+        <is>
+          <t>'-'</t>
+        </is>
+      </c>
+      <c r="AD13" t="inlineStr">
+        <is>
+          <t>Yes, 39.29% decrease in speed (from 14.0kts to 8.1kts)</t>
+        </is>
+      </c>
+      <c r="AE13" t="inlineStr">
+        <is>
+          <t>'-'</t>
+        </is>
+      </c>
+      <c r="AF13" t="inlineStr">
+        <is>
+          <t>'-'</t>
+        </is>
+      </c>
+      <c r="AG13" t="inlineStr">
+        <is>
+          <t>'-'</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>2025-3-Waverley-ReportAndAnnexes.pdf</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>gpt-4o-mini</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>1646</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Waverley Steam Navigation Co. Limited</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Brodick, Isle of Arran, Scotland</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>9.6kts</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>1947</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>24 injuries (21 passengers and 3 crew)</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>The engine stopping in a dead centre position</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>At the time of the accident there was a gentle westerly wind of 12kts (force 3), occasionally gusting to 21kts (force 5), and an air temperature of 17.7°C. The weather was sunny with little cloud.</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>The vessel’s deck and engineering crew were professional seafarers and at the time of the accident only the QM was a volunteer.</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="S14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="T14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>Yes, Waverley grounded on the edge of Boiler Reef, south of Sanda Island, Scotland in June 2004.</t>
+        </is>
+      </c>
+      <c r="V14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="W14" t="inlineStr">
+        <is>
+          <t>The operation, maintenance, and general husbandry of Waverley relied on the expertise of its crew and volunteers. There was no formal process to develop skills and knowledge.</t>
+        </is>
+      </c>
+      <c r="X14" t="inlineStr">
+        <is>
+          <t>1646</t>
+        </is>
+      </c>
+      <c r="Y14" t="inlineStr">
+        <is>
+          <t>213 (186 passengers and 27 crew)</t>
+        </is>
+      </c>
+      <c r="Z14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AA14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AB14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AC14" t="inlineStr">
+        <is>
+          <t>Clear, daylight, good visibility</t>
+        </is>
+      </c>
+      <c r="AD14" t="inlineStr">
+        <is>
+          <t>Yes, there was a reduction in speed. Normal operational speed was approximately 14.0 knots, and the speed decreased to 5.3 knots shortly before the accident. The percentage decrease in speed is approximately 62.14%.</t>
+        </is>
+      </c>
+      <c r="AE14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AF14" t="inlineStr">
+        <is>
+          <t>186 passengers (cargo weight not specified in tons or kilograms)</t>
+        </is>
+      </c>
+      <c r="AG14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>2025-3-Waverley-ReportAndAnnexes.pdf</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>gpt-4o-mini</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>1646</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Waverley Steam Navigation Co. Limited</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Brodick, Isle of Arran, Scotland</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>9.6kts</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>1947</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>At the time of the accident there was a gentle westerly wind of 12kts (force 3), occasionally gusting to 21kts (force 5), and an air temperature of 17.7°C. The weather was sunny with little cloud.</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="T15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>Yes, in June 2004, Waverley grounded on the edge of Boiler Reef, south of Sanda Island, Scotland.</t>
+        </is>
+      </c>
+      <c r="V15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="W15" t="inlineStr">
+        <is>
+          <t>The operation, maintenance, and general husbandry of Waverley relied on the expertise of its crew and volunteers.</t>
+        </is>
+      </c>
+      <c r="X15" t="inlineStr">
+        <is>
+          <t>1646</t>
+        </is>
+      </c>
+      <c r="Y15" t="inlineStr">
+        <is>
+          <t>213 (186 passengers and 27 crew)</t>
+        </is>
+      </c>
+      <c r="Z15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AA15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AB15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AC15" t="inlineStr">
+        <is>
+          <t>Clear, daylight, good visibility; -</t>
+        </is>
+      </c>
+      <c r="AD15" t="inlineStr">
+        <is>
+          <t>Yes, it decreased from 14.0kts to 5.3kts, which is approximately a 62.14% decrease.</t>
+        </is>
+      </c>
+      <c r="AE15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AF15" t="inlineStr">
+        <is>
+          <t>186 passengers (weight not provided in tons or kilograms).</t>
+        </is>
+      </c>
+      <c r="AG15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>2025-3-Waverley-ReportAndAnnexes.pdf</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>gpt-4o-mini</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>1646</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Waverley Steam Navigation Co. Limited</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Brodick, Isle of Arran, Scotland</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>9.6kts</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>1947</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>At the time of the accident there was a gentle westerly wind of 12kts (force 3), occasionally gusting to 21kts (force 5), and an air temperature of 17.7°C. High tide was 2.98m at 1409 and the predicted low tide was 0.63m at 1924. The weather was sunny with little cloud.</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="S16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="T16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="U16" t="inlineStr">
+        <is>
+          <t>Yes, Waverley grounded on the edge of Boiler Reef, south of Sanda Island, Scotland in June 2004.</t>
+        </is>
+      </c>
+      <c r="V16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="W16" t="inlineStr">
+        <is>
+          <t>The crew learned on-the-job, with little documented training provided beyond the safety induction and the management of specific hazards such as a fire on board.</t>
+        </is>
+      </c>
+      <c r="X16" t="inlineStr">
+        <is>
+          <t>1646</t>
+        </is>
+      </c>
+      <c r="Y16" t="inlineStr">
+        <is>
+          <t>213 (186 passengers and 27 crew)</t>
+        </is>
+      </c>
+      <c r="Z16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AA16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AB16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AC16" t="inlineStr">
+        <is>
+          <t>Clear, daylight, good visibility; wind variable but predominantly westerly force 3, gusting force 5</t>
+        </is>
+      </c>
+      <c r="AD16" t="inlineStr">
+        <is>
+          <t>Yes, the vessel's speed decreased from 9.6kts to 5.3kts, which is approximately a 44.79% decrease in speed</t>
+        </is>
+      </c>
+      <c r="AE16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AF16" t="inlineStr">
+        <is>
+          <t>186 passengers</t>
+        </is>
+      </c>
+      <c r="AG16" t="inlineStr">
         <is>
           <t>-</t>
         </is>

</xml_diff>